<commit_message>
in Monthly Reports please add 2 more fields Add/Edit forms and Import Excel format (2 test, 3 test and 4 test)
</commit_message>
<xml_diff>
--- a/public/assets/MonthlyReportSample1test.xlsx
+++ b/public/assets/MonthlyReportSample1test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t xml:space="preserve">Test Site</t>
   </si>
@@ -40,13 +40,16 @@
     <t xml:space="preserve">Site Unique Id</t>
   </si>
   <si>
+    <t xml:space="preserve">Tester Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is FLC*</t>
   </si>
   <si>
     <t xml:space="preserve">Does site do Recency Tests?*</t>
   </si>
   <si>
-    <t xml:space="preserve">Contact Number</t>
+    <t xml:space="preserve">Tester Contact Number</t>
   </si>
   <si>
     <t xml:space="preserve">Algorithm Type </t>
@@ -110,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">Eastern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -137,10 +143,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -254,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,44 +295,35 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X7" activeCellId="0" sqref="X7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +384,7 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -406,303 +401,85 @@
       </c>
       <c r="Z1" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
-        <v>30</v>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="I2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="L2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="8" t="n">
+        <v>34</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="8" t="n">
         <v>123</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="7" t="n">
+      <c r="O2" s="8"/>
+      <c r="P2" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="P2" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="Q2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="R2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="S2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="7" t="n">
+      <c r="T2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="V2" s="7" t="n">
+      <c r="W2" s="7" t="n">
         <v>2</v>
-      </c>
-      <c r="W2" s="7" t="n">
-        <v>0</v>
       </c>
       <c r="X2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="Y2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="Z2" s="7" t="n">
+      <c r="AA2" s="7" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Change some code login error page and monthly report pages
</commit_message>
<xml_diff>
--- a/public/assets/MonthlyReportSample1test.xlsx
+++ b/public/assets/MonthlyReportSample1test.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Test Kit Name1</t>
   </si>
   <si>
-    <t xml:space="preserve">Lot No 1</t>
+    <t xml:space="preserve">Lot No. 1</t>
   </si>
   <si>
     <t xml:space="preserve">Expiry Date 1</t>
@@ -297,31 +297,28 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Remove Facility from entire app
</commit_message>
<xml_diff>
--- a/public/assets/MonthlyReportSample1test.xlsx
+++ b/public/assets/MonthlyReportSample1test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t xml:space="preserve">Test Site</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">Site Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Facility</t>
-  </si>
-  <si>
     <t xml:space="preserve">Province </t>
   </si>
   <si>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve">Test Site Type1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility name 1</t>
   </si>
   <si>
     <t xml:space="preserve">Eastern</t>
@@ -312,13 +306,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -336,7 +333,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -381,7 +378,7 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -398,90 +395,84 @@
       </c>
       <c r="Z1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="K2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="L2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7" t="s">
+      <c r="M2" s="8" t="n">
+        <v>123</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="R2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="8" t="n">
-        <v>123</v>
-      </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="7" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>38</v>
+      <c r="U2" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="V2" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="W2" s="7" t="n">
         <v>0</v>
-      </c>
-      <c r="W2" s="7" t="n">
-        <v>2</v>
       </c>
       <c r="X2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="Y2" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z2" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="7" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>